<commit_message>
Update Python Code, Excel, PDF
to include analysis based on the months
</commit_message>
<xml_diff>
--- a/Cyclistic/fromPython.xlsx
+++ b/Cyclistic/fromPython.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apnat\Desktop\Cyclist Case Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apnat\Desktop\Summer\Cyclist Case Study\Cyclistic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0D6395-34B6-4AAE-8827-22DBBA858521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1211A1-57E5-4D8C-AFE8-98CE63728C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Statistics</t>
   </si>
@@ -110,6 +110,51 @@
   </si>
   <si>
     <t>Duration of Trips on</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Number of Trips on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High °C	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low °C	</t>
   </si>
 </sst>
 </file>
@@ -252,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +480,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,7 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -765,6 +816,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -810,7 +864,231 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="44">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -899,6 +1177,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9966"/>
+      <color rgb="FFFF6600"/>
       <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
@@ -2607,6 +2887,1921 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Duration of Trips by Month with Temp</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$Y$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Member</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$X$5:$X$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$Y$5:$Y$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1456447</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994747</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3478184</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3993104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2175925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3423706</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4862602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5363675</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4503565</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3305140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2287260</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AAD3-4D7D-B131-EF386AB0CBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$Z$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Casual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$X$5:$X$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$Z$5:$Z$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>277810</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>752145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3544105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5058883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3759011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6374637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11712154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10642635</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7276154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3835340</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2412159</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AAD3-4D7D-B131-EF386AB0CBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AA$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$X$5:$X$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AA$5:$AA$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1734257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2746892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7022289</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9051987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5934936</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9798359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16574756</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16006310</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11779719</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7140480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4699419</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AAD3-4D7D-B131-EF386AB0CBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1496461407"/>
+        <c:axId val="1496462655"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AB$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High °C	</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$X$5:$X$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AB$5:$AB$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AAD3-4D7D-B131-EF386AB0CBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AC$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low °C	</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$X$5:$X$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AC$5:$AC$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AAD3-4D7D-B131-EF386AB0CBE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1496443519"/>
+        <c:axId val="1496443103"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1496461407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496462655"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1496462655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496461407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1496443103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496443519"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1496443519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1496443103"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Number of Trips by Month with Temp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AF$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Member</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$AE$5:$AE$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AF$5:$AF$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>136075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>260005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>261718</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>188253</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>332645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>302218</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>243582</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>171592</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-31C3-4F0C-94CE-27E93C6B67D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AG$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Casual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$AE$5:$AE$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AG$5:$AG$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22854</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111530</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>159812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>86658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>154260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>268439</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>289071</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230346</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>144805</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>87985</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-31C3-4F0C-94CE-27E93C6B67D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AH$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$AE$5:$AE$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AH$5:$AH$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>143786</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>188967</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>371535</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>421530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>199990</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>342513</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550566</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>621716</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>532564</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>388387</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>259577</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-31C3-4F0C-94CE-27E93C6B67D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1496432287"/>
+        <c:axId val="1496422303"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AI$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High °C	</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$AE$5:$AE$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AI$5:$AI$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-31C3-4F0C-94CE-27E93C6B67D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fromPython!$AJ$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low °C	</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>fromPython!$AE$5:$AE$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fromPython!$AJ$5:$AJ$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-31C3-4F0C-94CE-27E93C6B67D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1496433119"/>
+        <c:axId val="1496431871"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1496432287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496422303"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1496422303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496432287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1496431871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1496433119"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1496433119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1496431871"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2727,6 +4922,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -4242,6 +6517,1012 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4379,6 +7660,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>289277</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6948</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>601486</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>155196</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C477CFBB-275D-FC9A-5BD0-CBEC372800CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>593209</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>296876</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142983</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D62DEE3-90B3-6B2A-6774-6F7F6768325D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4685,10 +8038,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C3:S17"/>
+  <dimension ref="C3:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="50" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4703,8 +8056,8 @@
     <col min="18" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:36" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="3:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -4741,8 +8094,44 @@
       <c r="S4" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="X4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ4" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -4779,8 +8168,44 @@
       <c r="S5" s="9">
         <v>10522595</v>
       </c>
+      <c r="X5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>1456447</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>277810</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>1734257</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="AC5" s="13">
+        <v>-9</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF5" s="6">
+        <v>136075</v>
+      </c>
+      <c r="AG5" s="6">
+        <v>7711</v>
+      </c>
+      <c r="AH5" s="9">
+        <v>143786</v>
+      </c>
+      <c r="AI5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="AJ5" s="13">
+        <v>-9</v>
+      </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
@@ -4817,8 +8242,44 @@
       <c r="S6" s="1">
         <v>10552467</v>
       </c>
+      <c r="X6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1994747</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>752145</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>2746892</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>-7</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>166113</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>22854</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>188967</v>
+      </c>
+      <c r="AI6" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="12">
+        <v>-7</v>
+      </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
@@ -4855,8 +8316,44 @@
       <c r="S7" s="1">
         <v>10596348</v>
       </c>
+      <c r="X7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>3478184</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>3544105</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>7022289</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>-1</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>260005</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>111530</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>371535</v>
+      </c>
+      <c r="AI7" s="12">
+        <v>8</v>
+      </c>
+      <c r="AJ7" s="12">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
@@ -4893,8 +8390,44 @@
       <c r="S8" s="1">
         <v>10774276</v>
       </c>
+      <c r="X8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>3993104</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>5058883</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>9051987</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>15</v>
+      </c>
+      <c r="AC8" s="12">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>261718</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>159812</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>421530</v>
+      </c>
+      <c r="AI8" s="12">
+        <v>15</v>
+      </c>
+      <c r="AJ8" s="12">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
@@ -4931,8 +8464,44 @@
       <c r="S9" s="1">
         <v>13237142</v>
       </c>
+      <c r="X9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>2175925</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>3759011</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>5934936</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>22</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>10</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>113332</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>86658</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>199990</v>
+      </c>
+      <c r="AI9" s="12">
+        <v>22</v>
+      </c>
+      <c r="AJ9" s="12">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
@@ -4969,8 +8538,44 @@
       <c r="S10" s="1">
         <v>19845583</v>
       </c>
+      <c r="X10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y10" s="6">
+        <v>3423706</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>6374637</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>9798359</v>
+      </c>
+      <c r="AB10" s="12">
+        <v>27</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>16</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF10" s="6">
+        <v>188253</v>
+      </c>
+      <c r="AG10" s="6">
+        <v>154260</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>342513</v>
+      </c>
+      <c r="AI10" s="12">
+        <v>27</v>
+      </c>
+      <c r="AJ10" s="12">
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
@@ -5007,8 +8612,44 @@
       <c r="S11" s="1">
         <v>16960989</v>
       </c>
+      <c r="X11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>4862602</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>11712154</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>16574756</v>
+      </c>
+      <c r="AB11" s="12">
+        <v>29</v>
+      </c>
+      <c r="AC11" s="12">
+        <v>19</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>282127</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>268439</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>550566</v>
+      </c>
+      <c r="AI11" s="12">
+        <v>29</v>
+      </c>
+      <c r="AJ11" s="12">
+        <v>19</v>
+      </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
@@ -5021,8 +8662,44 @@
       <c r="F12" s="1">
         <v>401786</v>
       </c>
+      <c r="X12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>5363675</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>10642635</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>16006310</v>
+      </c>
+      <c r="AB12" s="12">
+        <v>28</v>
+      </c>
+      <c r="AC12" s="12">
+        <v>18</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>332645</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>289071</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>621716</v>
+      </c>
+      <c r="AI12" s="12">
+        <v>28</v>
+      </c>
+      <c r="AJ12" s="12">
+        <v>18</v>
+      </c>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
@@ -5035,8 +8712,44 @@
       <c r="F13" s="1">
         <v>9.9918654730000007</v>
       </c>
+      <c r="X13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>4503565</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>7276154</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>11779719</v>
+      </c>
+      <c r="AB13" s="12">
+        <v>24</v>
+      </c>
+      <c r="AC13" s="12">
+        <v>14</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>302218</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>230346</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>532564</v>
+      </c>
+      <c r="AI13" s="12">
+        <v>24</v>
+      </c>
+      <c r="AJ13" s="12">
+        <v>14</v>
+      </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
@@ -5049,8 +8762,44 @@
       <c r="F14" s="1">
         <v>628322</v>
       </c>
+      <c r="X14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>3305140</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>3835340</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>7140480</v>
+      </c>
+      <c r="AB14" s="12">
+        <v>17</v>
+      </c>
+      <c r="AC14" s="12">
+        <v>7</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>243582</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>144805</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>388387</v>
+      </c>
+      <c r="AI14" s="12">
+        <v>17</v>
+      </c>
+      <c r="AJ14" s="12">
+        <v>7</v>
+      </c>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:36" x14ac:dyDescent="0.35">
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
@@ -5063,8 +8812,44 @@
       <c r="F15" s="1">
         <v>15.62550437</v>
       </c>
+      <c r="X15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>2287260</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>2412159</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>4699419</v>
+      </c>
+      <c r="AB15" s="12">
+        <v>9</v>
+      </c>
+      <c r="AC15" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>171592</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>87985</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>259577</v>
+      </c>
+      <c r="AI15" s="12">
+        <v>9</v>
+      </c>
+      <c r="AJ15" s="12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
@@ -5076,6 +8861,42 @@
       </c>
       <c r="F16" s="1">
         <v>2991023</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y16" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="12">
+        <v>-4</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF16" s="14">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="12">
+        <v>3</v>
+      </c>
+      <c r="AJ16" s="12">
+        <v>-4</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5094,51 +8915,139 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D17">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="43" priority="29">
       <formula>D5&lt;E5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="42" priority="30">
       <formula>D5&gt;E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:L11">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="41" priority="27">
       <formula>L5&lt;M5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="40" priority="28">
       <formula>L5&gt;M5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E17">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>E5&lt;D5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="38" priority="26">
       <formula>E5&gt;D5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M11">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="37" priority="23">
       <formula>M5&lt;L5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="36" priority="24">
       <formula>M5&gt;L5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q5:Q11">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="35" priority="21">
       <formula>Q5&lt;R5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="34" priority="22">
       <formula>Q5&gt;R5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:R11">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="33" priority="19">
       <formula>R5&lt;Q5</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="32" priority="20">
+      <formula>R5&gt;Q5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB5:AC16">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF9966"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI5:AJ16">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF9966"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y5:Y9">
+    <cfRule type="expression" dxfId="19" priority="15">
+      <formula>Y5&lt;Z5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="16">
+      <formula>Y5&gt;Z5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z5:Z9">
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>Z5&lt;Y5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="14">
+      <formula>Z5&gt;Y5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y10:Y16">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>Y10&lt;Z10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>Y10&gt;Z10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z10:Z16">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>Z10&lt;Y10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>Z10&gt;Y10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF5:AF9">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>AF5&lt;AG5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>AF5&gt;AG5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG5:AG9">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>AG5&lt;AF5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AG5&gt;AF5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10:AF16">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>AF10&lt;AG10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AF10&gt;AG10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG10:AG16">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AG10&lt;AF10</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>R5&gt;Q5</formula>
+      <formula>AG10&gt;AF10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>